<commit_message>
Added Article Number element
</commit_message>
<xml_diff>
--- a/preserve-standard-metadata.xlsx
+++ b/preserve-standard-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Lehigh\Work From Home\Spreadsheet\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09532EBB-F442-432E-97A1-1592AC394C89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1447F3D6-25B3-4152-A65C-757F8783F0D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="789" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="789" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Islandora Metadata Template" sheetId="1" r:id="rId1"/>
@@ -1264,7 +1264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="1243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="1244">
   <si>
     <t>Title</t>
   </si>
@@ -4993,6 +4993,9 @@
   </si>
   <si>
     <t>Preferred-Citation</t>
+  </si>
+  <si>
+    <t>Article-Number</t>
   </si>
 </sst>
 </file>
@@ -5606,10 +5609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BO1"/>
+  <dimension ref="A1:BP1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AM5" sqref="AM5"/>
+    <sheetView tabSelected="1" topLeftCell="BC1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BN13" sqref="BN13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5648,13 +5651,13 @@
     <col min="53" max="56" width="25.7109375" customWidth="1"/>
     <col min="57" max="61" width="23.28515625" customWidth="1"/>
     <col min="63" max="63" width="16.28515625" customWidth="1"/>
-    <col min="64" max="64" width="13.140625" customWidth="1"/>
-    <col min="65" max="65" width="19.7109375" customWidth="1"/>
-    <col min="66" max="66" width="16.85546875" customWidth="1"/>
-    <col min="67" max="67" width="20.5703125" customWidth="1"/>
+    <col min="64" max="65" width="13.140625" customWidth="1"/>
+    <col min="66" max="66" width="19.7109375" customWidth="1"/>
+    <col min="67" max="67" width="16.85546875" customWidth="1"/>
+    <col min="68" max="68" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:68" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
@@ -5847,13 +5850,16 @@
       <c r="BL1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="BM1" s="8" t="s">
+      <c r="BM1" s="5" t="s">
+        <v>1243</v>
+      </c>
+      <c r="BN1" s="8" t="s">
         <v>1156</v>
       </c>
-      <c r="BN1" s="8" t="s">
+      <c r="BO1" s="8" t="s">
         <v>1157</v>
       </c>
-      <c r="BO1" s="8" t="s">
+      <c r="BP1" s="8" t="s">
         <v>1158</v>
       </c>
     </row>
@@ -11169,46 +11175,46 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B114:B115"/>
-    <mergeCell ref="B122:B123"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="B112:B113"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="B525:B526"/>
+    <mergeCell ref="B542:B543"/>
+    <mergeCell ref="B458:B459"/>
+    <mergeCell ref="B485:B486"/>
+    <mergeCell ref="B438:B439"/>
+    <mergeCell ref="B440:B441"/>
+    <mergeCell ref="B410:B411"/>
+    <mergeCell ref="B412:B413"/>
+    <mergeCell ref="B359:B360"/>
+    <mergeCell ref="B391:B392"/>
+    <mergeCell ref="B334:B335"/>
+    <mergeCell ref="B341:B342"/>
+    <mergeCell ref="B321:B322"/>
+    <mergeCell ref="B332:B333"/>
+    <mergeCell ref="B307:B308"/>
+    <mergeCell ref="B312:B313"/>
+    <mergeCell ref="B250:B251"/>
+    <mergeCell ref="B298:B299"/>
+    <mergeCell ref="B218:B219"/>
+    <mergeCell ref="B234:B235"/>
+    <mergeCell ref="B192:B193"/>
+    <mergeCell ref="B214:B215"/>
+    <mergeCell ref="B175:B176"/>
+    <mergeCell ref="B177:B178"/>
     <mergeCell ref="B160:B161"/>
     <mergeCell ref="B162:B163"/>
     <mergeCell ref="B146:B147"/>
     <mergeCell ref="B152:B153"/>
     <mergeCell ref="B132:B133"/>
     <mergeCell ref="B139:B140"/>
-    <mergeCell ref="B218:B219"/>
-    <mergeCell ref="B234:B235"/>
-    <mergeCell ref="B192:B193"/>
-    <mergeCell ref="B214:B215"/>
-    <mergeCell ref="B175:B176"/>
-    <mergeCell ref="B177:B178"/>
-    <mergeCell ref="B321:B322"/>
-    <mergeCell ref="B332:B333"/>
-    <mergeCell ref="B307:B308"/>
-    <mergeCell ref="B312:B313"/>
-    <mergeCell ref="B250:B251"/>
-    <mergeCell ref="B298:B299"/>
-    <mergeCell ref="B410:B411"/>
-    <mergeCell ref="B412:B413"/>
-    <mergeCell ref="B359:B360"/>
-    <mergeCell ref="B391:B392"/>
-    <mergeCell ref="B334:B335"/>
-    <mergeCell ref="B341:B342"/>
-    <mergeCell ref="B525:B526"/>
-    <mergeCell ref="B542:B543"/>
-    <mergeCell ref="B458:B459"/>
-    <mergeCell ref="B485:B486"/>
-    <mergeCell ref="B438:B439"/>
-    <mergeCell ref="B440:B441"/>
+    <mergeCell ref="B122:B123"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="B112:B113"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B114:B115"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11284,7 +11290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E33B95ED-AE6D-4843-B48F-1891A5A7A8D7}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q34" sqref="Q34"/>
     </sheetView>

</xml_diff>

<commit_message>
Added fields present in XSL template
</commit_message>
<xml_diff>
--- a/preserve-standard-metadata.xlsx
+++ b/preserve-standard-metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20385"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Lehigh\Work From Home\Spreadsheet\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Islandora\Spreadsheet Ingest\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1447F3D6-25B3-4152-A65C-757F8783F0D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841BE325-E84D-4DEA-A821-462100A4874A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="789" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -302,7 +302,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{A45955F0-C447-4E97-A7BA-BD50D6CFDEEA}">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{A45955F0-C447-4E97-A7BA-BD50D6CFDEEA}">
       <text>
         <r>
           <rPr>
@@ -328,7 +328,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{454DE92F-D709-4465-BBD9-0A87F9FE3884}">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{454DE92F-D709-4465-BBD9-0A87F9FE3884}">
       <text>
         <r>
           <rPr>
@@ -355,7 +355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{B54B678A-3085-4E00-B156-EEE7F291535C}">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{B54B678A-3085-4E00-B156-EEE7F291535C}">
       <text>
         <r>
           <rPr>
@@ -380,7 +380,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{63A938D5-DD9F-4C28-85B7-862F01C2557B}">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{63A938D5-DD9F-4C28-85B7-862F01C2557B}">
       <text>
         <r>
           <rPr>
@@ -406,7 +406,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{F3FC3F32-7AD5-4AD5-BC96-E284BC31D639}">
+    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{F3FC3F32-7AD5-4AD5-BC96-E284BC31D639}">
       <text>
         <r>
           <rPr>
@@ -433,7 +433,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{C8C7F5BA-7F77-486D-89C1-EE8841EBF865}">
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{C8C7F5BA-7F77-486D-89C1-EE8841EBF865}">
       <text>
         <r>
           <rPr>
@@ -459,7 +459,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{67119DCC-AF6E-4126-84BC-791CAF171D86}">
+    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{67119DCC-AF6E-4126-84BC-791CAF171D86}">
       <text>
         <r>
           <rPr>
@@ -484,7 +484,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{E3B509DE-43E9-44B5-BDEC-98F9565127F8}">
+    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{E3B509DE-43E9-44B5-BDEC-98F9565127F8}">
       <text>
         <r>
           <rPr>
@@ -508,7 +508,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{E2CC8CA8-D47F-4EEC-A37F-5713BAB9E324}">
+    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{E2CC8CA8-D47F-4EEC-A37F-5713BAB9E324}">
       <text>
         <r>
           <rPr>
@@ -532,7 +532,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{091FF495-4462-4CC1-8F23-39AEEA05BB0A}">
+    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{091FF495-4462-4CC1-8F23-39AEEA05BB0A}">
       <text>
         <r>
           <rPr>
@@ -558,7 +558,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{E08F8DEB-76A8-4E0E-966F-F84105839B5D}">
+    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{E08F8DEB-76A8-4E0E-966F-F84105839B5D}">
       <text>
         <r>
           <rPr>
@@ -582,7 +582,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{B0E91B56-1822-41AF-A6F9-757BE53B78B3}">
+    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{B0E91B56-1822-41AF-A6F9-757BE53B78B3}">
       <text>
         <r>
           <rPr>
@@ -609,7 +609,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{C37A58A6-F5F3-40F1-A828-7C18B781422F}">
+    <comment ref="AD1" authorId="0" shapeId="0" xr:uid="{C37A58A6-F5F3-40F1-A828-7C18B781422F}">
       <text>
         <r>
           <rPr>
@@ -635,7 +635,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{3991E12B-3A71-4A97-B3B5-1180C0193E47}">
+    <comment ref="AE1" authorId="0" shapeId="0" xr:uid="{3991E12B-3A71-4A97-B3B5-1180C0193E47}">
       <text>
         <r>
           <rPr>
@@ -661,7 +661,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0" shapeId="0" xr:uid="{85E6D484-5A90-45DD-9A06-ACAEA4E36301}">
+    <comment ref="AF1" authorId="0" shapeId="0" xr:uid="{85E6D484-5A90-45DD-9A06-ACAEA4E36301}">
       <text>
         <r>
           <rPr>
@@ -687,7 +687,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0" shapeId="0" xr:uid="{F6F51BBE-97C7-4474-9B6A-5F28B5E6742F}">
+    <comment ref="AG1" authorId="0" shapeId="0" xr:uid="{F6F51BBE-97C7-4474-9B6A-5F28B5E6742F}">
       <text>
         <r>
           <rPr>
@@ -712,7 +712,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0" shapeId="0" xr:uid="{4BBD92AC-9B74-421C-B77E-49175DBE1818}">
+    <comment ref="AH1" authorId="0" shapeId="0" xr:uid="{4BBD92AC-9B74-421C-B77E-49175DBE1818}">
       <text>
         <r>
           <rPr>
@@ -738,7 +738,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0" shapeId="0" xr:uid="{A13F7FB5-2D79-4361-A957-990F73831417}">
+    <comment ref="AI1" authorId="0" shapeId="0" xr:uid="{A13F7FB5-2D79-4361-A957-990F73831417}">
       <text>
         <r>
           <rPr>
@@ -763,7 +763,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0" shapeId="0" xr:uid="{6FFEBC39-3422-4FA0-98D2-223893A185AA}">
+    <comment ref="AJ1" authorId="0" shapeId="0" xr:uid="{6FFEBC39-3422-4FA0-98D2-223893A185AA}">
       <text>
         <r>
           <rPr>
@@ -789,7 +789,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0" shapeId="0" xr:uid="{5D40D71D-7BB4-4B93-99E1-B2FD752A62E9}">
+    <comment ref="AK1" authorId="0" shapeId="0" xr:uid="{5D40D71D-7BB4-4B93-99E1-B2FD752A62E9}">
       <text>
         <r>
           <rPr>
@@ -818,7 +818,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0" shapeId="0" xr:uid="{FC850D2C-B335-4894-B732-C94221F61B96}">
+    <comment ref="AL1" authorId="0" shapeId="0" xr:uid="{FC850D2C-B335-4894-B732-C94221F61B96}">
       <text>
         <r>
           <rPr>
@@ -843,7 +843,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0" shapeId="0" xr:uid="{2B000DB6-660D-4091-9425-D687C9E4C607}">
+    <comment ref="AM1" authorId="0" shapeId="0" xr:uid="{2B000DB6-660D-4091-9425-D687C9E4C607}">
       <text>
         <r>
           <rPr>
@@ -868,7 +868,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0" shapeId="0" xr:uid="{ACE9F1BF-C616-4680-8DBD-DF6BFB8D98FC}">
+    <comment ref="AP1" authorId="0" shapeId="0" xr:uid="{ACE9F1BF-C616-4680-8DBD-DF6BFB8D98FC}">
       <text>
         <r>
           <rPr>
@@ -893,7 +893,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO1" authorId="0" shapeId="0" xr:uid="{3C8AC224-C308-41F9-9AF6-DC71515D8098}">
+    <comment ref="AQ1" authorId="0" shapeId="0" xr:uid="{3C8AC224-C308-41F9-9AF6-DC71515D8098}">
       <text>
         <r>
           <rPr>
@@ -923,7 +923,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP1" authorId="0" shapeId="0" xr:uid="{5C0A6C82-6B8A-4ADD-AA15-F5F27C7C9B16}">
+    <comment ref="AR1" authorId="0" shapeId="0" xr:uid="{5C0A6C82-6B8A-4ADD-AA15-F5F27C7C9B16}">
       <text>
         <r>
           <rPr>
@@ -948,7 +948,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS1" authorId="0" shapeId="0" xr:uid="{795F82C3-4195-4E48-981C-501ABEED3CA8}">
+    <comment ref="AU1" authorId="0" shapeId="0" xr:uid="{795F82C3-4195-4E48-981C-501ABEED3CA8}">
       <text>
         <r>
           <rPr>
@@ -977,7 +977,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW1" authorId="0" shapeId="0" xr:uid="{B17F5182-5CD6-471A-802B-B04940EB1F07}">
+    <comment ref="AY1" authorId="0" shapeId="0" xr:uid="{B17F5182-5CD6-471A-802B-B04940EB1F07}">
       <text>
         <r>
           <rPr>
@@ -1004,7 +1004,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX1" authorId="0" shapeId="0" xr:uid="{6FA6BCB2-96AD-42FE-B85A-93E824A4B205}">
+    <comment ref="AZ1" authorId="0" shapeId="0" xr:uid="{6FA6BCB2-96AD-42FE-B85A-93E824A4B205}">
       <text>
         <r>
           <rPr>
@@ -1029,7 +1029,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AY1" authorId="0" shapeId="0" xr:uid="{83A64A19-0D57-4885-9A2C-DFE6B3D0CF3A}">
+    <comment ref="BA1" authorId="0" shapeId="0" xr:uid="{83A64A19-0D57-4885-9A2C-DFE6B3D0CF3A}">
       <text>
         <r>
           <rPr>
@@ -1056,7 +1056,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AZ1" authorId="0" shapeId="0" xr:uid="{C23793B6-57EA-4BE5-9374-0C67D52D0D5C}">
+    <comment ref="BB1" authorId="0" shapeId="0" xr:uid="{C23793B6-57EA-4BE5-9374-0C67D52D0D5C}">
       <text>
         <r>
           <rPr>
@@ -1083,7 +1083,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BA1" authorId="0" shapeId="0" xr:uid="{4500A268-EF31-4F3C-9D7B-2CBB70B9E291}">
+    <comment ref="BC1" authorId="0" shapeId="0" xr:uid="{4500A268-EF31-4F3C-9D7B-2CBB70B9E291}">
       <text>
         <r>
           <rPr>
@@ -1109,7 +1109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BE1" authorId="0" shapeId="0" xr:uid="{6E8A1D6E-E9E7-4730-96F4-42FCA2E3B89E}">
+    <comment ref="BG1" authorId="0" shapeId="0" xr:uid="{6E8A1D6E-E9E7-4730-96F4-42FCA2E3B89E}">
       <text>
         <r>
           <rPr>
@@ -1134,7 +1134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BG1" authorId="0" shapeId="0" xr:uid="{8F72E90C-4BED-4038-997E-A10E8E8AA220}">
+    <comment ref="BI1" authorId="0" shapeId="0" xr:uid="{8F72E90C-4BED-4038-997E-A10E8E8AA220}">
       <text>
         <r>
           <rPr>
@@ -1159,7 +1159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BH1" authorId="0" shapeId="0" xr:uid="{7D7262B2-604D-4B7F-8CCD-D4AD1EB59919}">
+    <comment ref="BJ1" authorId="0" shapeId="0" xr:uid="{7D7262B2-604D-4B7F-8CCD-D4AD1EB59919}">
       <text>
         <r>
           <rPr>
@@ -1184,7 +1184,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BJ1" authorId="0" shapeId="0" xr:uid="{8903C426-306A-4610-8322-B47368832A22}">
+    <comment ref="BM1" authorId="0" shapeId="0" xr:uid="{8903C426-306A-4610-8322-B47368832A22}">
       <text>
         <r>
           <rPr>
@@ -1209,7 +1209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BK1" authorId="0" shapeId="0" xr:uid="{581ADCAD-C33E-4E29-A328-0CB4CAFA8386}">
+    <comment ref="BN1" authorId="0" shapeId="0" xr:uid="{581ADCAD-C33E-4E29-A328-0CB4CAFA8386}">
       <text>
         <r>
           <rPr>
@@ -1234,7 +1234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BL1" authorId="0" shapeId="0" xr:uid="{2D74D483-8099-47E3-BB22-E0D0F1C8457F}">
+    <comment ref="BO1" authorId="0" shapeId="0" xr:uid="{2D74D483-8099-47E3-BB22-E0D0F1C8457F}">
       <text>
         <r>
           <rPr>
@@ -1264,7 +1264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="1244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="1247">
   <si>
     <t>Title</t>
   </si>
@@ -4996,6 +4996,15 @@
   </si>
   <si>
     <t>Article-Number</t>
+  </si>
+  <si>
+    <t>Advisors</t>
+  </si>
+  <si>
+    <t>Embargo-Date</t>
+  </si>
+  <si>
+    <t>Report-Number</t>
   </si>
 </sst>
 </file>
@@ -5266,7 +5275,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -5328,6 +5337,7 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5609,10 +5619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BP1"/>
+  <dimension ref="A1:BS1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BN13" sqref="BN13"/>
+    <sheetView tabSelected="1" topLeftCell="BG1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BS27" sqref="BS27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5628,36 +5638,36 @@
     <col min="10" max="10" width="15.5703125" customWidth="1"/>
     <col min="11" max="11" width="22.85546875" customWidth="1"/>
     <col min="12" max="13" width="19.42578125" customWidth="1"/>
-    <col min="14" max="15" width="12.85546875" customWidth="1"/>
-    <col min="18" max="18" width="12.28515625" customWidth="1"/>
-    <col min="19" max="19" width="17.42578125" customWidth="1"/>
-    <col min="20" max="20" width="22" customWidth="1"/>
-    <col min="21" max="21" width="17.85546875" style="23" customWidth="1"/>
-    <col min="22" max="25" width="17.85546875" style="2" customWidth="1"/>
-    <col min="26" max="27" width="10.140625" customWidth="1"/>
-    <col min="28" max="29" width="14.42578125" customWidth="1"/>
-    <col min="30" max="31" width="11.140625" customWidth="1"/>
-    <col min="32" max="32" width="14.5703125" customWidth="1"/>
-    <col min="33" max="33" width="11.5703125" customWidth="1"/>
-    <col min="34" max="35" width="14.42578125" customWidth="1"/>
-    <col min="36" max="40" width="19.140625" customWidth="1"/>
-    <col min="41" max="41" width="18.5703125" customWidth="1"/>
-    <col min="42" max="42" width="16.7109375" customWidth="1"/>
-    <col min="43" max="43" width="13.85546875" customWidth="1"/>
-    <col min="44" max="44" width="12" customWidth="1"/>
-    <col min="49" max="50" width="16.140625" customWidth="1"/>
-    <col min="51" max="51" width="13.7109375" customWidth="1"/>
-    <col min="52" max="52" width="19.140625" customWidth="1"/>
-    <col min="53" max="56" width="25.7109375" customWidth="1"/>
-    <col min="57" max="61" width="23.28515625" customWidth="1"/>
-    <col min="63" max="63" width="16.28515625" customWidth="1"/>
-    <col min="64" max="65" width="13.140625" customWidth="1"/>
-    <col min="66" max="66" width="19.7109375" customWidth="1"/>
-    <col min="67" max="67" width="16.85546875" customWidth="1"/>
-    <col min="68" max="68" width="20.5703125" customWidth="1"/>
+    <col min="14" max="16" width="12.85546875" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" customWidth="1"/>
+    <col min="20" max="20" width="17.42578125" customWidth="1"/>
+    <col min="21" max="21" width="22" customWidth="1"/>
+    <col min="22" max="23" width="17.85546875" style="23" customWidth="1"/>
+    <col min="24" max="27" width="17.85546875" style="2" customWidth="1"/>
+    <col min="28" max="29" width="10.140625" customWidth="1"/>
+    <col min="30" max="31" width="14.42578125" customWidth="1"/>
+    <col min="32" max="33" width="11.140625" customWidth="1"/>
+    <col min="34" max="34" width="14.5703125" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" customWidth="1"/>
+    <col min="36" max="37" width="14.42578125" customWidth="1"/>
+    <col min="38" max="42" width="19.140625" customWidth="1"/>
+    <col min="43" max="43" width="18.5703125" customWidth="1"/>
+    <col min="44" max="44" width="16.7109375" customWidth="1"/>
+    <col min="45" max="45" width="13.85546875" customWidth="1"/>
+    <col min="46" max="46" width="12" customWidth="1"/>
+    <col min="51" max="52" width="16.140625" customWidth="1"/>
+    <col min="53" max="53" width="13.7109375" customWidth="1"/>
+    <col min="54" max="54" width="19.140625" customWidth="1"/>
+    <col min="55" max="58" width="25.7109375" customWidth="1"/>
+    <col min="59" max="64" width="23.28515625" customWidth="1"/>
+    <col min="66" max="66" width="16.28515625" customWidth="1"/>
+    <col min="67" max="68" width="13.140625" customWidth="1"/>
+    <col min="69" max="69" width="19.7109375" customWidth="1"/>
+    <col min="70" max="70" width="16.85546875" customWidth="1"/>
+    <col min="71" max="71" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:71" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
@@ -5701,165 +5711,174 @@
         <v>2</v>
       </c>
       <c r="O1" s="5" t="s">
+        <v>1244</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>1164</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>1142</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>1143</v>
       </c>
-      <c r="U1" s="22" t="s">
+      <c r="V1" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="31" t="s">
+        <v>1245</v>
+      </c>
+      <c r="X1" s="6" t="s">
         <v>1166</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="Y1" s="19" t="s">
+      <c r="AA1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>1147</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>1148</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AI1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>1149</v>
       </c>
-      <c r="AK1" s="8" t="s">
+      <c r="AM1" s="8" t="s">
         <v>1150</v>
       </c>
-      <c r="AL1" s="8" t="s">
+      <c r="AN1" s="8" t="s">
         <v>1173</v>
       </c>
-      <c r="AM1" s="8" t="s">
+      <c r="AO1" s="8" t="s">
         <v>1242</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AP1" s="5" t="s">
         <v>1168</v>
       </c>
-      <c r="AO1" s="8" t="s">
+      <c r="AQ1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>1161</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>1159</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>1160</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AT1" s="8" t="s">
+      <c r="AV1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AU1" s="8" t="s">
+      <c r="AW1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AV1" s="8" t="s">
+      <c r="AX1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="AY1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AX1" s="20" t="s">
+      <c r="AZ1" s="20" t="s">
         <v>1151</v>
       </c>
-      <c r="AY1" s="3" t="s">
+      <c r="BA1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="BB1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="BA1" s="5" t="s">
+      <c r="BC1" s="5" t="s">
         <v>1152</v>
       </c>
-      <c r="BB1" s="5" t="s">
+      <c r="BD1" s="5" t="s">
         <v>1153</v>
       </c>
-      <c r="BC1" s="5" t="s">
+      <c r="BE1" s="5" t="s">
         <v>1154</v>
       </c>
-      <c r="BD1" s="5" t="s">
+      <c r="BF1" s="5" t="s">
         <v>1163</v>
       </c>
-      <c r="BE1" s="5" t="s">
+      <c r="BG1" s="5" t="s">
         <v>1155</v>
       </c>
-      <c r="BF1" s="5" t="s">
+      <c r="BH1" s="5" t="s">
         <v>1162</v>
       </c>
-      <c r="BG1" s="5" t="s">
+      <c r="BI1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="BH1" s="3" t="s">
+      <c r="BJ1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="BI1" s="8" t="s">
+      <c r="BK1" s="8" t="s">
         <v>1165</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BL1" s="8" t="s">
+        <v>1246</v>
+      </c>
+      <c r="BM1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="BK1" s="5" t="s">
+      <c r="BN1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="BL1" s="5" t="s">
+      <c r="BO1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="BM1" s="5" t="s">
+      <c r="BP1" s="5" t="s">
         <v>1243</v>
       </c>
-      <c r="BN1" s="8" t="s">
+      <c r="BQ1" s="8" t="s">
         <v>1156</v>
       </c>
-      <c r="BO1" s="8" t="s">
+      <c r="BR1" s="8" t="s">
         <v>1157</v>
       </c>
-      <c r="BP1" s="8" t="s">
+      <c r="BS1" s="8" t="s">
         <v>1158</v>
       </c>
     </row>
@@ -5881,25 +5900,25 @@
           <x14:formula1>
             <xm:f>'Type list'!$A$1:$A$11</xm:f>
           </x14:formula1>
-          <xm:sqref>P2:P1048576</xm:sqref>
+          <xm:sqref>Q2:Q1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{220336D5-88C8-43FC-BAAF-0F62C8E76DFF}">
           <x14:formula1>
             <xm:f>'Date-Qualifier list'!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>T2:T1048576</xm:sqref>
+          <xm:sqref>U2:U1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8D7091BA-978E-46FA-96E4-C1D3C047EB93}">
           <x14:formula1>
             <xm:f>'Digital-Origin list'!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>AI2:AI1048576</xm:sqref>
+          <xm:sqref>AK2:AK1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0775DFD4-8502-4F27-ACAE-32EBE7E704B0}">
           <x14:formula1>
             <xm:f>'Capture-Device list'!$A$1:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>AO2:AO1048576</xm:sqref>
+          <xm:sqref>AQ2:AQ1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4B785CF6-50BB-4D62-B1E7-6D2B06C23EE6}">
           <x14:formula1>
@@ -5911,19 +5930,19 @@
           <x14:formula1>
             <xm:f>'Language list'!$B$2:$B$548</xm:f>
           </x14:formula1>
-          <xm:sqref>AC1:AC1048576</xm:sqref>
+          <xm:sqref>AE1:AE1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D6EEDB1A-39A3-466A-BD21-575AA8E1C06B}">
           <x14:formula1>
             <xm:f>Departments!$A$2:$A$51</xm:f>
           </x14:formula1>
-          <xm:sqref>O1:O1048576</xm:sqref>
+          <xm:sqref>P1:P1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{32216E77-359A-4520-92EA-8DFCC393471E}">
           <x14:formula1>
             <xm:f>'Language list'!A2:A548</xm:f>
           </x14:formula1>
-          <xm:sqref>AB1:AB1048576</xm:sqref>
+          <xm:sqref>AD1:AD1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6020,7 +6039,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A15">
+  <sortState ref="A1:A15">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11175,46 +11194,46 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B114:B115"/>
+    <mergeCell ref="B122:B123"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="B112:B113"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="B160:B161"/>
+    <mergeCell ref="B162:B163"/>
+    <mergeCell ref="B146:B147"/>
+    <mergeCell ref="B152:B153"/>
+    <mergeCell ref="B132:B133"/>
+    <mergeCell ref="B139:B140"/>
+    <mergeCell ref="B218:B219"/>
+    <mergeCell ref="B234:B235"/>
+    <mergeCell ref="B192:B193"/>
+    <mergeCell ref="B214:B215"/>
+    <mergeCell ref="B175:B176"/>
+    <mergeCell ref="B177:B178"/>
+    <mergeCell ref="B321:B322"/>
+    <mergeCell ref="B332:B333"/>
+    <mergeCell ref="B307:B308"/>
+    <mergeCell ref="B312:B313"/>
+    <mergeCell ref="B250:B251"/>
+    <mergeCell ref="B298:B299"/>
+    <mergeCell ref="B410:B411"/>
+    <mergeCell ref="B412:B413"/>
+    <mergeCell ref="B359:B360"/>
+    <mergeCell ref="B391:B392"/>
+    <mergeCell ref="B334:B335"/>
+    <mergeCell ref="B341:B342"/>
     <mergeCell ref="B525:B526"/>
     <mergeCell ref="B542:B543"/>
     <mergeCell ref="B458:B459"/>
     <mergeCell ref="B485:B486"/>
     <mergeCell ref="B438:B439"/>
     <mergeCell ref="B440:B441"/>
-    <mergeCell ref="B410:B411"/>
-    <mergeCell ref="B412:B413"/>
-    <mergeCell ref="B359:B360"/>
-    <mergeCell ref="B391:B392"/>
-    <mergeCell ref="B334:B335"/>
-    <mergeCell ref="B341:B342"/>
-    <mergeCell ref="B321:B322"/>
-    <mergeCell ref="B332:B333"/>
-    <mergeCell ref="B307:B308"/>
-    <mergeCell ref="B312:B313"/>
-    <mergeCell ref="B250:B251"/>
-    <mergeCell ref="B298:B299"/>
-    <mergeCell ref="B218:B219"/>
-    <mergeCell ref="B234:B235"/>
-    <mergeCell ref="B192:B193"/>
-    <mergeCell ref="B214:B215"/>
-    <mergeCell ref="B175:B176"/>
-    <mergeCell ref="B177:B178"/>
-    <mergeCell ref="B160:B161"/>
-    <mergeCell ref="B162:B163"/>
-    <mergeCell ref="B146:B147"/>
-    <mergeCell ref="B152:B153"/>
-    <mergeCell ref="B132:B133"/>
-    <mergeCell ref="B139:B140"/>
-    <mergeCell ref="B122:B123"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="B112:B113"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B114:B115"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11358,7 +11377,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B6">
+  <sortState ref="A2:B6">
     <sortCondition ref="A1:A6"/>
   </sortState>
   <hyperlinks>

</xml_diff>